<commit_message>
Implement card pool. Separated card pool from card build operation
</commit_message>
<xml_diff>
--- a/cards_description/graveyard.xlsx
+++ b/cards_description/graveyard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Змеевик</t>
   </si>
@@ -196,13 +196,181 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Creature</t>
   </si>
   <si>
     <t>Zmeevik</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Kosoglyad</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Undead</t>
+  </si>
+  <si>
+    <t>Necro</t>
+  </si>
+  <si>
+    <t>Askola</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Rumol</t>
+  </si>
+  <si>
+    <t>Warlock</t>
+  </si>
+  <si>
+    <t>Ghoul</t>
+  </si>
+  <si>
+    <t>Trupnik</t>
+  </si>
+  <si>
+    <t>Vargula</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Deck</t>
+  </si>
+  <si>
+    <t>Debtor's sword</t>
+  </si>
+  <si>
+    <t>DeckType</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>WeaponType</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Blood Sphere</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>Transplanta</t>
+  </si>
+  <si>
+    <t>Crypt staff</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Undead dawn</t>
+  </si>
+  <si>
+    <t>Scroll</t>
+  </si>
+  <si>
+    <t>DamageType</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Magical</t>
+  </si>
+  <si>
+    <t>ScrollUser</t>
+  </si>
+  <si>
+    <t>Posion Rain</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>1_2</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Ядовитый дождь</t>
+  </si>
+  <si>
+    <t>Кидает яд 1 урон 2 хода на всех героев соперника</t>
+  </si>
+  <si>
+    <t>Сломанное копье</t>
+  </si>
+  <si>
+    <t>Копье</t>
+  </si>
+  <si>
+    <t>Broken spear</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Rotten shield</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Noble mantle</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>ArmorValue</t>
+  </si>
+  <si>
+    <t>Rotten sword</t>
+  </si>
+  <si>
+    <t>Posion Spit</t>
+  </si>
+  <si>
+    <t>1_1</t>
+  </si>
+  <si>
+    <t>Scroll's return</t>
+  </si>
+  <si>
+    <t>Flesh summon</t>
+  </si>
+  <si>
+    <t>Heal</t>
   </si>
 </sst>
 </file>
@@ -326,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -373,6 +541,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -687,19 +856,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -710,21 +885,560 @@
         <v>52</v>
       </c>
       <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
       </c>
       <c r="D2">
         <v>6</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" t="s">
+        <v>87</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>104</v>
+      </c>
+      <c r="K16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" t="s">
+        <v>87</v>
+      </c>
+      <c r="L19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" t="s">
+        <v>93</v>
+      </c>
+      <c r="N21" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +1451,7 @@
   <dimension ref="B2:O26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1750,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="17">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>5</v>
@@ -1064,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H31"/>
+  <dimension ref="B3:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,7 +1803,7 @@
         <v>48</v>
       </c>
       <c r="H3" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1158,6 +1872,12 @@
         <v>9</v>
       </c>
       <c r="D11" s="11"/>
+      <c r="G11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="8">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
@@ -1167,6 +1887,10 @@
       <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
@@ -1176,6 +1900,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="11"/>
+      <c r="G13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
@@ -1185,6 +1913,12 @@
         <v>1</v>
       </c>
       <c r="D14" s="11"/>
+      <c r="G14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
@@ -1192,16 +1926,26 @@
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="11"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G15" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="10">
+        <v>14</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1209,29 +1953,53 @@
       <c r="D20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="15">
+        <v>3</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="17">
+        <v>1</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>43</v>
       </c>
@@ -1240,7 +2008,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>33</v>
       </c>
@@ -1251,7 +2019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +2028,7 @@
       </c>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +2037,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>46</v>
       </c>

</xml_diff>